<commit_message>
automatic adding of seats and total energy usage to my df
</commit_message>
<xml_diff>
--- a/overall/data/Aircraft Databank v2.xlsx
+++ b/overall/data/Aircraft Databank v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRohr\Desktop\Masterarbeit\Python\overall\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667F50C0-D9A0-4760-90F1-F40059CEA313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A83193E-FC02-4B73-89BA-C524FF326D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="1" xr2:uid="{B2B150D8-E64E-4875-9280-D2B2D82F52FA}"/>
+    <workbookView xWindow="-75" yWindow="0" windowWidth="9750" windowHeight="10155" firstSheet="1" activeTab="1" xr2:uid="{B2B150D8-E64E-4875-9280-D2B2D82F52FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Table" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="314">
   <si>
     <t>Company</t>
   </si>
@@ -984,6 +984,21 @@
   </si>
   <si>
     <t xml:space="preserve">B767-200/ER/EM                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC9-40                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC9-10                         </t>
+  </si>
+  <si>
+    <t>B707-300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC9-50                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1011-500                   </t>
   </si>
 </sst>
 </file>
@@ -1442,8 +1457,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R64"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
@@ -4005,18 +4020,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7E994-12F2-4962-AF8C-42BF75C864FA}">
-  <dimension ref="A1:AA186"/>
+  <dimension ref="A1:AA189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="49" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X123" sqref="X123"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B183" sqref="B183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
     <col min="2" max="2" width="20.2265625" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" customWidth="1"/>
-    <col min="4" max="7" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" hidden="1" customWidth="1"/>
+    <col min="4" max="7" width="16.81640625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="16.08984375" customWidth="1"/>
     <col min="9" max="9" width="13.26953125" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
@@ -4059,9 +4074,7 @@
       <c r="J1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="21" t="s">
-        <v>276</v>
-      </c>
+      <c r="K1" s="21"/>
       <c r="L1" s="1" t="s">
         <v>269</v>
       </c>
@@ -14042,7 +14055,7 @@
         <v>16</v>
       </c>
       <c r="B181" t="s">
-        <v>51</v>
+        <v>312</v>
       </c>
       <c r="C181">
         <v>146</v>
@@ -14084,7 +14097,7 @@
         <v>53</v>
       </c>
       <c r="B182" t="s">
-        <v>54</v>
+        <v>313</v>
       </c>
       <c r="C182">
         <v>141</v>
@@ -14168,7 +14181,7 @@
         <v>16</v>
       </c>
       <c r="B184" t="s">
-        <v>59</v>
+        <v>309</v>
       </c>
       <c r="C184">
         <v>113</v>
@@ -14208,7 +14221,7 @@
         <v>28</v>
       </c>
       <c r="B185" t="s">
-        <v>62</v>
+        <v>310</v>
       </c>
       <c r="C185">
         <v>98</v>
@@ -14284,6 +14297,64 @@
         <v>102</v>
       </c>
       <c r="X186" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="187" spans="1:24">
+      <c r="A187" t="s">
+        <v>10</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="I187" s="5">
+        <v>15.8095</v>
+      </c>
+      <c r="J187" s="5">
+        <v>0.41126000000000001</v>
+      </c>
+      <c r="W187" t="s">
+        <v>102</v>
+      </c>
+      <c r="X187" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="188" spans="1:24">
+      <c r="A188" t="s">
+        <v>4</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H188" s="5">
+        <v>28.176500000000001</v>
+      </c>
+      <c r="I188" s="5">
+        <v>15.8095</v>
+      </c>
+      <c r="J188" s="5"/>
+      <c r="W188" t="s">
+        <v>102</v>
+      </c>
+      <c r="X188" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="189" spans="1:24">
+      <c r="A189" t="s">
+        <v>10</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H189" s="5">
+        <v>27.027799999999999</v>
+      </c>
+      <c r="W189" t="s">
+        <v>102</v>
+      </c>
+      <c r="X189" t="s">
         <v>254</v>
       </c>
     </row>

</xml_diff>